<commit_message>
Type hinting and comments (#13)
* fixing all the type errors

* tweaking sample data

* fix return

* desperation

* fixing test

* removing extra function

* fmt lint
</commit_message>
<xml_diff>
--- a/tests/sample_data.xlsx
+++ b/tests/sample_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\Stuff\Logic\Financial\240106 Spending Tracking\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\Stuff\Logic\Coding Projects\spending-tracking\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03EB0322-4FAE-43C3-AEF4-40BCAFC73AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E4816B-DB8E-4380-A2D8-318A29C0866D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9EFDC7C0-B3BA-4261-B230-5BB77DCF9D87}"/>
   </bookViews>
@@ -603,7 +603,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45296</v>
+        <v>45293</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>

</xml_diff>